<commit_message>
remove composite timestamp fields that had been added to the dataset (which combined date and time fields); update data dictionaries, and add data dictionary automation script
</commit_message>
<xml_diff>
--- a/SMARTS/Data_Dictionaries/Stormwater_EnforcementActions_DataDictionary.xlsx
+++ b/SMARTS/Data_Dictionaries/Stormwater_EnforcementActions_DataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\David\Stormwater\_SMARTS_Data_Download_Automation\Data_Dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/CA_data_portal/SMARTS/Data_Dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263048F3-4580-44A1-898B-71A15D665DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{263048F3-4580-44A1-898B-71A15D665DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{426BB998-D208-4909-89EC-59417A9BBE78}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{73A369D3-E501-4417-A57B-32D283C67892}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73A369D3-E501-4417-A57B-32D283C67892}"/>
   </bookViews>
   <sheets>
     <sheet name="Enforcement_Actions" sheetId="7" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="211">
   <si>
     <t>Field Title</t>
   </si>
@@ -693,6 +693,20 @@
   </si>
   <si>
     <t>Name of the regulated facility/site.</t>
+  </si>
+  <si>
+    <t>Regional Water Quality Control Board office that has primary responsibility for regulation of the facility: 
+- 1: North Coast
+- 2: San Francisco Bay
+- 3: Central Coast
+- 4: Los Angeles
+- 5F: Central Valley (Fresno)
+- 5R: Central Valley (Redding)
+- 5S: Central Valley (Sacramento)
+- 6: Lahontan
+- 7: Colorado River
+- 8: Santa Ana
+- 9: San Diego</t>
   </si>
 </sst>
 </file>
@@ -896,47 +910,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1006,10 +1019,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1047,7 +1064,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1153,7 +1170,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1295,7 +1312,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1303,785 +1320,648 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9B1353-0134-449B-8A87-2DB58E793A23}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="103.7109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="103.6640625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="b">
-        <f>E2=A2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="b">
-        <f t="shared" ref="F3:F42" si="0">E3=A3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="F4" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="F5" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="F6" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>113</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="18" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F7" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="18" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F8" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="F9" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="17" t="s">
+      <c r="D10" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="D11" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="C12" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F10" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="17" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="F11" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" s="17" t="s">
+      <c r="D27" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D35" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="C40" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D40" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F12" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="18" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="C41" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F13" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="18" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="C42" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F14" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="F15" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="F16" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="F17" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F18" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="F28" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="F29" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F31" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="F38" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="F39" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F40" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F41" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F42" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-    </row>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="B50:B1048576 B1:B42">
+  <conditionalFormatting sqref="C1:C42 C50:C1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"numeric"</formula>
     </cfRule>
@@ -2093,7 +1973,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B42" xr:uid="{4E0F304F-3107-4AAF-A837-F7B5281CC604}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C42" xr:uid="{4E0F304F-3107-4AAF-A837-F7B5281CC604}">
       <formula1>"text, numeric, timestamp"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2106,26 +1986,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F306A2E-7B02-41D2-88BA-37E362374F49}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17" style="22" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="59" style="22" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17" style="21" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="59" style="21" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="26" style="11" customWidth="1"/>
-    <col min="12" max="12" width="63.5703125" style="11" customWidth="1"/>
-    <col min="15" max="17" width="22.5703125" customWidth="1"/>
-    <col min="18" max="18" width="80.28515625" customWidth="1"/>
+    <col min="9" max="11" width="26" customWidth="1"/>
+    <col min="12" max="12" width="63.5546875" customWidth="1"/>
+    <col min="15" max="17" width="22.5546875" customWidth="1"/>
+    <col min="18" max="18" width="80.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -2172,23 +2052,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:18" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="12" t="str" cm="1">
+      <c r="B2" s="11" t="str" cm="1">
         <f t="array" ref="B2">IF(IFERROR(IFERROR(INDEX(J:J,$F2),INDEX(Q:Q,$G2)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F2),INDEX(Q:Q,$G2)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C2" s="13" t="str" cm="1">
+      <c r="C2" s="12" t="str" cm="1">
         <f t="array" ref="C2">IF(IFERROR(IFERROR(INDEX(K:K,$F2),INDEX(O:O,$G2)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F2),INDEX(O:O,$G2)),"-"))</f>
         <v>Waste Discharge ID</v>
       </c>
-      <c r="D2" s="12" t="str" cm="1">
+      <c r="D2" s="11" t="str" cm="1">
         <f t="array" ref="D2">IF(IFERROR(IFERROR(INDEX(L:L,$F2),INDEX(R:R,$G2)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F2),INDEX(R:R,$G2)),"-"))</f>
@@ -2202,7 +2082,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="1">
-        <f>MATCH(E2,P:P,0)</f>
+        <f t="shared" ref="G2:G43" si="1">MATCH(E2,P:P,0)</f>
         <v>13</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -2230,23 +2110,23 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:18" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="str" cm="1">
+      <c r="B3" s="11" t="str" cm="1">
         <f t="array" ref="B3">IF(IFERROR(IFERROR(INDEX(J:J,$F3),INDEX(Q:Q,$G3)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F3),INDEX(Q:Q,$G3)),"-"))</f>
         <v>Number</v>
       </c>
-      <c r="C3" s="13" t="str" cm="1">
+      <c r="C3" s="12" t="str" cm="1">
         <f t="array" ref="C3">IF(IFERROR(IFERROR(INDEX(K:K,$F3),INDEX(O:O,$G3)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F3),INDEX(O:O,$G3)),"-"))</f>
         <v>Regulatory Measure ID (Application ID)</v>
       </c>
-      <c r="D3" s="12" t="str" cm="1">
+      <c r="D3" s="11" t="str" cm="1">
         <f t="array" ref="D3">IF(IFERROR(IFERROR(INDEX(L:L,$F3),INDEX(R:R,$G3)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F3),INDEX(R:R,$G3)),"-"))</f>
@@ -2260,7 +2140,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="e">
-        <f>MATCH(E3,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -2288,23 +2168,23 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="12" t="str" cm="1">
+      <c r="B4" s="11" t="str" cm="1">
         <f t="array" ref="B4">IF(IFERROR(IFERROR(INDEX(J:J,$F4),INDEX(Q:Q,$G4)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F4),INDEX(Q:Q,$G4)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C4" s="13" t="str" cm="1">
+      <c r="C4" s="12" t="str" cm="1">
         <f t="array" ref="C4">IF(IFERROR(IFERROR(INDEX(K:K,$F4),INDEX(O:O,$G4)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F4),INDEX(O:O,$G4)),"-"))</f>
         <v>Enforcement ID</v>
       </c>
-      <c r="D4" s="12" t="str" cm="1">
+      <c r="D4" s="11" t="str" cm="1">
         <f t="array" ref="D4">IF(IFERROR(IFERROR(INDEX(L:L,$F4),INDEX(R:R,$G4)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F4),INDEX(R:R,$G4)),"-"))</f>
@@ -2318,7 +2198,7 @@
         <v>#N/A</v>
       </c>
       <c r="G4" s="1">
-        <f>MATCH(E4,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -2346,23 +2226,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="12" t="str" cm="1">
+      <c r="B5" s="11" t="str" cm="1">
         <f t="array" ref="B5">IF(IFERROR(IFERROR(INDEX(J:J,$F5),INDEX(Q:Q,$G5)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F5),INDEX(Q:Q,$G5)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C5" s="13" t="str" cm="1">
+      <c r="C5" s="12" t="str" cm="1">
         <f t="array" ref="C5">IF(IFERROR(IFERROR(INDEX(K:K,$F5),INDEX(O:O,$G5)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F5),INDEX(O:O,$G5)),"-"))</f>
         <v>Enforcement Type</v>
       </c>
-      <c r="D5" s="12" t="str" cm="1">
+      <c r="D5" s="11" t="str" cm="1">
         <f t="array" ref="D5">IF(IFERROR(IFERROR(INDEX(L:L,$F5),INDEX(R:R,$G5)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F5),INDEX(R:R,$G5)),"-"))</f>
@@ -2376,7 +2256,7 @@
         <v>#N/A</v>
       </c>
       <c r="G5" s="1">
-        <f>MATCH(E5,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -2400,23 +2280,23 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:18" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="12" t="str" cm="1">
+      <c r="B6" s="11" t="str" cm="1">
         <f t="array" ref="B6">IF(IFERROR(IFERROR(INDEX(J:J,$F6),INDEX(Q:Q,$G6)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F6),INDEX(Q:Q,$G6)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C6" s="13" t="str" cm="1">
+      <c r="C6" s="12" t="str" cm="1">
         <f t="array" ref="C6">IF(IFERROR(IFERROR(INDEX(K:K,$F6),INDEX(O:O,$G6)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F6),INDEX(O:O,$G6)),"-"))</f>
         <v>Enforcement Status</v>
       </c>
-      <c r="D6" s="12" t="str" cm="1">
+      <c r="D6" s="11" t="str" cm="1">
         <f t="array" ref="D6">IF(IFERROR(IFERROR(INDEX(L:L,$F6),INDEX(R:R,$G6)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F6),INDEX(R:R,$G6)),"-"))</f>
@@ -2430,7 +2310,7 @@
         <v>#N/A</v>
       </c>
       <c r="G6" s="1">
-        <f>MATCH(E6,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I6" s="7" t="s">
@@ -2458,23 +2338,23 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="12" t="str" cm="1">
+      <c r="B7" s="11" t="str" cm="1">
         <f t="array" ref="B7">IF(IFERROR(IFERROR(INDEX(J:J,$F7),INDEX(Q:Q,$G7)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F7),INDEX(Q:Q,$G7)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C7" s="13" t="str" cm="1">
+      <c r="C7" s="12" t="str" cm="1">
         <f t="array" ref="C7">IF(IFERROR(IFERROR(INDEX(K:K,$F7),INDEX(O:O,$G7)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F7),INDEX(O:O,$G7)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D7" s="12" t="str" cm="1">
+      <c r="D7" s="11" t="str" cm="1">
         <f t="array" ref="D7">IF(IFERROR(IFERROR(INDEX(L:L,$F7),INDEX(R:R,$G7)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F7),INDEX(R:R,$G7)),"-"))</f>
@@ -2488,7 +2368,7 @@
         <v>#N/A</v>
       </c>
       <c r="G7" s="1" t="e">
-        <f>MATCH(E7,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I7" s="6" t="s">
@@ -2510,23 +2390,23 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:18" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="12" t="str" cm="1">
+      <c r="B8" s="11" t="str" cm="1">
         <f t="array" ref="B8">IF(IFERROR(IFERROR(INDEX(J:J,$F8),INDEX(Q:Q,$G8)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F8),INDEX(Q:Q,$G8)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C8" s="13" t="str" cm="1">
+      <c r="C8" s="12" t="str" cm="1">
         <f t="array" ref="C8">IF(IFERROR(IFERROR(INDEX(K:K,$F8),INDEX(O:O,$G8)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F8),INDEX(O:O,$G8)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D8" s="12" t="str" cm="1">
+      <c r="D8" s="11" t="str" cm="1">
         <f t="array" ref="D8">IF(IFERROR(IFERROR(INDEX(L:L,$F8),INDEX(R:R,$G8)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F8),INDEX(R:R,$G8)),"-"))</f>
@@ -2540,7 +2420,7 @@
         <v>#N/A</v>
       </c>
       <c r="G8" s="1" t="e">
-        <f>MATCH(E8,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -2568,23 +2448,23 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="12" t="str" cm="1">
+      <c r="B9" s="11" t="str" cm="1">
         <f t="array" ref="B9">IF(IFERROR(IFERROR(INDEX(J:J,$F9),INDEX(Q:Q,$G9)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F9),INDEX(Q:Q,$G9)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C9" s="13" t="str" cm="1">
+      <c r="C9" s="12" t="str" cm="1">
         <f t="array" ref="C9">IF(IFERROR(IFERROR(INDEX(K:K,$F9),INDEX(O:O,$G9)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F9),INDEX(O:O,$G9)),"-"))</f>
         <v>Enforcement Description</v>
       </c>
-      <c r="D9" s="12" t="str" cm="1">
+      <c r="D9" s="11" t="str" cm="1">
         <f t="array" ref="D9">IF(IFERROR(IFERROR(INDEX(L:L,$F9),INDEX(R:R,$G9)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F9),INDEX(R:R,$G9)),"-"))</f>
@@ -2598,7 +2478,7 @@
         <v>#N/A</v>
       </c>
       <c r="G9" s="1">
-        <f>MATCH(E9,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="I9" s="8" t="s">
@@ -2626,23 +2506,23 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="12" t="str" cm="1">
+      <c r="B10" s="11" t="str" cm="1">
         <f t="array" ref="B10">IF(IFERROR(IFERROR(INDEX(J:J,$F10),INDEX(Q:Q,$G10)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F10),INDEX(Q:Q,$G10)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C10" s="13" t="str" cm="1">
+      <c r="C10" s="12" t="str" cm="1">
         <f t="array" ref="C10">IF(IFERROR(IFERROR(INDEX(K:K,$F10),INDEX(O:O,$G10)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F10),INDEX(O:O,$G10)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D10" s="12" t="str" cm="1">
+      <c r="D10" s="11" t="str" cm="1">
         <f t="array" ref="D10">IF(IFERROR(IFERROR(INDEX(L:L,$F10),INDEX(R:R,$G10)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F10),INDEX(R:R,$G10)),"-"))</f>
@@ -2656,7 +2536,7 @@
         <v>#N/A</v>
       </c>
       <c r="G10" s="1" t="e">
-        <f>MATCH(E10,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I10" s="6" t="s">
@@ -2684,24 +2564,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="12" t="str" cm="1">
+      <c r="B11" s="11" t="str" cm="1">
         <f t="array" ref="B11">IF(IFERROR(IFERROR(INDEX(J:J,$F11),INDEX(Q:Q,$G11)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F11),INDEX(Q:Q,$G11)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C11" s="13" t="str" cm="1">
+      <c r="C11" s="12" t="str" cm="1">
         <f t="array" ref="C11">IF(IFERROR(IFERROR(INDEX(K:K,$F11),INDEX(O:O,$G11)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F11),INDEX(O:O,$G11)),"-"))</f>
         <v>Order/Resolution
 Number</v>
       </c>
-      <c r="D11" s="12" t="str" cm="1">
+      <c r="D11" s="11" t="str" cm="1">
         <f t="array" ref="D11">IF(IFERROR(IFERROR(INDEX(L:L,$F11),INDEX(R:R,$G11)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F11),INDEX(R:R,$G11)),"-"))</f>
@@ -2715,7 +2595,7 @@
         <v>#N/A</v>
       </c>
       <c r="G11" s="1">
-        <f>MATCH(E11,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -2743,23 +2623,23 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="12" t="str" cm="1">
+      <c r="B12" s="11" t="str" cm="1">
         <f t="array" ref="B12">IF(IFERROR(IFERROR(INDEX(J:J,$F12),INDEX(Q:Q,$G12)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F12),INDEX(Q:Q,$G12)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C12" s="13" t="str" cm="1">
+      <c r="C12" s="12" t="str" cm="1">
         <f t="array" ref="C12">IF(IFERROR(IFERROR(INDEX(K:K,$F12),INDEX(O:O,$G12)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F12),INDEX(O:O,$G12)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D12" s="12" t="str" cm="1">
+      <c r="D12" s="11" t="str" cm="1">
         <f t="array" ref="D12">IF(IFERROR(IFERROR(INDEX(L:L,$F12),INDEX(R:R,$G12)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F12),INDEX(R:R,$G12)),"-"))</f>
@@ -2773,7 +2653,7 @@
         <v>#N/A</v>
       </c>
       <c r="G12" s="1" t="e">
-        <f>MATCH(E12,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I12" s="8" t="s">
@@ -2801,23 +2681,23 @@
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="12" t="str" cm="1">
+      <c r="B13" s="11" t="str" cm="1">
         <f t="array" ref="B13">IF(IFERROR(IFERROR(INDEX(J:J,$F13),INDEX(Q:Q,$G13)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F13),INDEX(Q:Q,$G13)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C13" s="13" t="str" cm="1">
+      <c r="C13" s="12" t="str" cm="1">
         <f t="array" ref="C13">IF(IFERROR(IFERROR(INDEX(K:K,$F13),INDEX(O:O,$G13)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F13),INDEX(O:O,$G13)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D13" s="12" t="str" cm="1">
+      <c r="D13" s="11" t="str" cm="1">
         <f t="array" ref="D13">IF(IFERROR(IFERROR(INDEX(L:L,$F13),INDEX(R:R,$G13)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F13),INDEX(R:R,$G13)),"-"))</f>
@@ -2831,7 +2711,7 @@
         <v>#N/A</v>
       </c>
       <c r="G13" s="1" t="e">
-        <f>MATCH(E13,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -2853,23 +2733,23 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="12" t="str" cm="1">
+      <c r="B14" s="11" t="str" cm="1">
         <f t="array" ref="B14">IF(IFERROR(IFERROR(INDEX(J:J,$F14),INDEX(Q:Q,$G14)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F14),INDEX(Q:Q,$G14)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C14" s="13" t="str" cm="1">
+      <c r="C14" s="12" t="str" cm="1">
         <f t="array" ref="C14">IF(IFERROR(IFERROR(INDEX(K:K,$F14),INDEX(O:O,$G14)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F14),INDEX(O:O,$G14)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D14" s="12" t="str" cm="1">
+      <c r="D14" s="11" t="str" cm="1">
         <f t="array" ref="D14">IF(IFERROR(IFERROR(INDEX(L:L,$F14),INDEX(R:R,$G14)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F14),INDEX(R:R,$G14)),"-"))</f>
@@ -2883,7 +2763,7 @@
         <v>#N/A</v>
       </c>
       <c r="G14" s="1" t="e">
-        <f>MATCH(E14,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I14" s="8" t="s">
@@ -2911,23 +2791,23 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:18" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="12" t="str" cm="1">
+      <c r="B15" s="11" t="str" cm="1">
         <f t="array" ref="B15">IF(IFERROR(IFERROR(INDEX(J:J,$F15),INDEX(Q:Q,$G15)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F15),INDEX(Q:Q,$G15)),"-"))</f>
         <v>Money</v>
       </c>
-      <c r="C15" s="13" t="str" cm="1">
+      <c r="C15" s="12" t="str" cm="1">
         <f t="array" ref="C15">IF(IFERROR(IFERROR(INDEX(K:K,$F15),INDEX(O:O,$G15)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F15),INDEX(O:O,$G15)),"-"))</f>
         <v>Initial Assessed Amount</v>
       </c>
-      <c r="D15" s="12" t="str" cm="1">
+      <c r="D15" s="11" t="str" cm="1">
         <f t="array" ref="D15">IF(IFERROR(IFERROR(INDEX(L:L,$F15),INDEX(R:R,$G15)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F15),INDEX(R:R,$G15)),"-"))</f>
@@ -2941,7 +2821,7 @@
         <v>#N/A</v>
       </c>
       <c r="G15" s="1">
-        <f>MATCH(E15,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -2969,23 +2849,23 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:18" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="12" t="str" cm="1">
+      <c r="B16" s="11" t="str" cm="1">
         <f t="array" ref="B16">IF(IFERROR(IFERROR(INDEX(J:J,$F16),INDEX(Q:Q,$G16)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F16),INDEX(Q:Q,$G16)),"-"))</f>
         <v>Money</v>
       </c>
-      <c r="C16" s="13" t="str" cm="1">
+      <c r="C16" s="12" t="str" cm="1">
         <f t="array" ref="C16">IF(IFERROR(IFERROR(INDEX(K:K,$F16),INDEX(O:O,$G16)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F16),INDEX(O:O,$G16)),"-"))</f>
         <v>Total Assessment Amount</v>
       </c>
-      <c r="D16" s="12" t="str" cm="1">
+      <c r="D16" s="11" t="str" cm="1">
         <f t="array" ref="D16">IF(IFERROR(IFERROR(INDEX(L:L,$F16),INDEX(R:R,$G16)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F16),INDEX(R:R,$G16)),"-"))</f>
@@ -2999,7 +2879,7 @@
         <v>#N/A</v>
       </c>
       <c r="G16" s="1">
-        <f>MATCH(E16,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="I16" s="6" t="s">
@@ -3027,23 +2907,23 @@
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="12" t="str" cm="1">
+      <c r="B17" s="11" t="str" cm="1">
         <f t="array" ref="B17">IF(IFERROR(IFERROR(INDEX(J:J,$F17),INDEX(Q:Q,$G17)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F17),INDEX(Q:Q,$G17)),"-"))</f>
         <v>Money</v>
       </c>
-      <c r="C17" s="13" t="str" cm="1">
+      <c r="C17" s="12" t="str" cm="1">
         <f t="array" ref="C17">IF(IFERROR(IFERROR(INDEX(K:K,$F17),INDEX(O:O,$G17)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F17),INDEX(O:O,$G17)),"-"))</f>
         <v>Liability $ Paid</v>
       </c>
-      <c r="D17" s="12" t="str" cm="1">
+      <c r="D17" s="11" t="str" cm="1">
         <f t="array" ref="D17">IF(IFERROR(IFERROR(INDEX(L:L,$F17),INDEX(R:R,$G17)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F17),INDEX(R:R,$G17)),"-"))</f>
@@ -3057,7 +2937,7 @@
         <v>#N/A</v>
       </c>
       <c r="G17" s="1">
-        <f>MATCH(E17,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I17" s="6" t="s">
@@ -3085,23 +2965,23 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="12" t="str" cm="1">
+      <c r="B18" s="11" t="str" cm="1">
         <f t="array" ref="B18">IF(IFERROR(IFERROR(INDEX(J:J,$F18),INDEX(Q:Q,$G18)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F18),INDEX(Q:Q,$G18)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C18" s="13" t="str" cm="1">
+      <c r="C18" s="12" t="str" cm="1">
         <f t="array" ref="C18">IF(IFERROR(IFERROR(INDEX(K:K,$F18),INDEX(O:O,$G18)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F18),INDEX(O:O,$G18)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D18" s="12" t="str" cm="1">
+      <c r="D18" s="11" t="str" cm="1">
         <f t="array" ref="D18">IF(IFERROR(IFERROR(INDEX(L:L,$F18),INDEX(R:R,$G18)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F18),INDEX(R:R,$G18)),"-"))</f>
@@ -3115,7 +2995,7 @@
         <v>#N/A</v>
       </c>
       <c r="G18" s="1" t="e">
-        <f>MATCH(E18,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I18" s="6" t="s">
@@ -3143,23 +3023,23 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="12" t="str" cm="1">
+      <c r="B19" s="11" t="str" cm="1">
         <f t="array" ref="B19">IF(IFERROR(IFERROR(INDEX(J:J,$F19),INDEX(Q:Q,$G19)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F19),INDEX(Q:Q,$G19)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C19" s="13" t="str" cm="1">
+      <c r="C19" s="12" t="str" cm="1">
         <f t="array" ref="C19">IF(IFERROR(IFERROR(INDEX(K:K,$F19),INDEX(O:O,$G19)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F19),INDEX(O:O,$G19)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D19" s="12" t="str" cm="1">
+      <c r="D19" s="11" t="str" cm="1">
         <f t="array" ref="D19">IF(IFERROR(IFERROR(INDEX(L:L,$F19),INDEX(R:R,$G19)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F19),INDEX(R:R,$G19)),"-"))</f>
@@ -3173,7 +3053,7 @@
         <v>#N/A</v>
       </c>
       <c r="G19" s="1" t="e">
-        <f>MATCH(E19,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I19" s="8" t="s">
@@ -3201,23 +3081,23 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="12" t="str" cm="1">
+      <c r="B20" s="11" t="str" cm="1">
         <f t="array" ref="B20">IF(IFERROR(IFERROR(INDEX(J:J,$F20),INDEX(Q:Q,$G20)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F20),INDEX(Q:Q,$G20)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C20" s="13" t="str" cm="1">
+      <c r="C20" s="12" t="str" cm="1">
         <f t="array" ref="C20">IF(IFERROR(IFERROR(INDEX(K:K,$F20),INDEX(O:O,$G20)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F20),INDEX(O:O,$G20)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D20" s="12" t="str" cm="1">
+      <c r="D20" s="11" t="str" cm="1">
         <f t="array" ref="D20">IF(IFERROR(IFERROR(INDEX(L:L,$F20),INDEX(R:R,$G20)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F20),INDEX(R:R,$G20)),"-"))</f>
@@ -3231,10 +3111,10 @@
         <v>#N/A</v>
       </c>
       <c r="G20" s="1" t="e">
-        <f>MATCH(E20,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I20" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I20" s="13" t="s">
         <v>49</v>
       </c>
       <c r="J20" s="5"/>
@@ -3253,23 +3133,23 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="12" t="str" cm="1">
+      <c r="B21" s="11" t="str" cm="1">
         <f t="array" ref="B21">IF(IFERROR(IFERROR(INDEX(J:J,$F21),INDEX(Q:Q,$G21)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F21),INDEX(Q:Q,$G21)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C21" s="13" t="str" cm="1">
+      <c r="C21" s="12" t="str" cm="1">
         <f t="array" ref="C21">IF(IFERROR(IFERROR(INDEX(K:K,$F21),INDEX(O:O,$G21)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F21),INDEX(O:O,$G21)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D21" s="12" t="str" cm="1">
+      <c r="D21" s="11" t="str" cm="1">
         <f t="array" ref="D21">IF(IFERROR(IFERROR(INDEX(L:L,$F21),INDEX(R:R,$G21)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F21),INDEX(R:R,$G21)),"-"))</f>
@@ -3283,10 +3163,10 @@
         <v>#N/A</v>
       </c>
       <c r="G21" s="1" t="e">
-        <f>MATCH(E21,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I21" s="15" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I21" s="14" t="s">
         <v>50</v>
       </c>
       <c r="J21" s="5"/>
@@ -3305,23 +3185,23 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="12" t="str" cm="1">
+      <c r="B22" s="11" t="str" cm="1">
         <f t="array" ref="B22">IF(IFERROR(IFERROR(INDEX(J:J,$F22),INDEX(Q:Q,$G22)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F22),INDEX(Q:Q,$G22)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C22" s="13" t="str" cm="1">
+      <c r="C22" s="12" t="str" cm="1">
         <f t="array" ref="C22">IF(IFERROR(IFERROR(INDEX(K:K,$F22),INDEX(O:O,$G22)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F22),INDEX(O:O,$G22)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D22" s="12" t="str" cm="1">
+      <c r="D22" s="11" t="str" cm="1">
         <f t="array" ref="D22">IF(IFERROR(IFERROR(INDEX(L:L,$F22),INDEX(R:R,$G22)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F22),INDEX(R:R,$G22)),"-"))</f>
@@ -3335,10 +3215,10 @@
         <v>#N/A</v>
       </c>
       <c r="G22" s="1" t="e">
-        <f>MATCH(E22,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I22" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I22" s="13" t="s">
         <v>51</v>
       </c>
       <c r="J22" s="5"/>
@@ -3357,23 +3237,23 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+    <row r="23" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="12" t="str" cm="1">
+      <c r="B23" s="11" t="str" cm="1">
         <f t="array" ref="B23">IF(IFERROR(IFERROR(INDEX(J:J,$F23),INDEX(Q:Q,$G23)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F23),INDEX(Q:Q,$G23)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C23" s="13" t="str" cm="1">
+      <c r="C23" s="12" t="str" cm="1">
         <f t="array" ref="C23">IF(IFERROR(IFERROR(INDEX(K:K,$F23),INDEX(O:O,$G23)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F23),INDEX(O:O,$G23)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D23" s="12" t="str" cm="1">
+      <c r="D23" s="11" t="str" cm="1">
         <f t="array" ref="D23">IF(IFERROR(IFERROR(INDEX(L:L,$F23),INDEX(R:R,$G23)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F23),INDEX(R:R,$G23)),"-"))</f>
@@ -3387,10 +3267,10 @@
         <v>#N/A</v>
       </c>
       <c r="G23" s="1" t="e">
-        <f>MATCH(E23,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I23" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I23" s="13" t="s">
         <v>52</v>
       </c>
       <c r="J23" s="5"/>
@@ -3409,23 +3289,23 @@
         <v>197</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+    <row r="24" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="12" t="str" cm="1">
+      <c r="B24" s="11" t="str" cm="1">
         <f t="array" ref="B24">IF(IFERROR(IFERROR(INDEX(J:J,$F24),INDEX(Q:Q,$G24)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F24),INDEX(Q:Q,$G24)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C24" s="13" t="str" cm="1">
+      <c r="C24" s="12" t="str" cm="1">
         <f t="array" ref="C24">IF(IFERROR(IFERROR(INDEX(K:K,$F24),INDEX(O:O,$G24)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F24),INDEX(O:O,$G24)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D24" s="12" t="str" cm="1">
+      <c r="D24" s="11" t="str" cm="1">
         <f t="array" ref="D24">IF(IFERROR(IFERROR(INDEX(L:L,$F24),INDEX(R:R,$G24)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F24),INDEX(R:R,$G24)),"-"))</f>
@@ -3439,10 +3319,10 @@
         <v>#N/A</v>
       </c>
       <c r="G24" s="1" t="e">
-        <f>MATCH(E24,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I24" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>53</v>
       </c>
       <c r="J24" s="5"/>
@@ -3461,23 +3341,23 @@
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
+    <row r="25" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="12" t="str" cm="1">
+      <c r="B25" s="11" t="str" cm="1">
         <f t="array" ref="B25">IF(IFERROR(IFERROR(INDEX(J:J,$F25),INDEX(Q:Q,$G25)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F25),INDEX(Q:Q,$G25)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C25" s="13" t="str" cm="1">
+      <c r="C25" s="12" t="str" cm="1">
         <f t="array" ref="C25">IF(IFERROR(IFERROR(INDEX(K:K,$F25),INDEX(O:O,$G25)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F25),INDEX(O:O,$G25)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D25" s="12" t="str" cm="1">
+      <c r="D25" s="11" t="str" cm="1">
         <f t="array" ref="D25">IF(IFERROR(IFERROR(INDEX(L:L,$F25),INDEX(R:R,$G25)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F25),INDEX(R:R,$G25)),"-"))</f>
@@ -3491,7 +3371,7 @@
         <v>#N/A</v>
       </c>
       <c r="G25" s="1" t="e">
-        <f>MATCH(E25,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I25" s="8" t="s">
@@ -3519,23 +3399,23 @@
         <v>199</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+    <row r="26" spans="1:18" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="12" t="str" cm="1">
+      <c r="B26" s="11" t="str" cm="1">
         <f t="array" ref="B26">IF(IFERROR(IFERROR(INDEX(J:J,$F26),INDEX(Q:Q,$G26)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F26),INDEX(Q:Q,$G26)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C26" s="13" t="str" cm="1">
+      <c r="C26" s="12" t="str" cm="1">
         <f t="array" ref="C26">IF(IFERROR(IFERROR(INDEX(K:K,$F26),INDEX(O:O,$G26)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F26),INDEX(O:O,$G26)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D26" s="12" t="str" cm="1">
+      <c r="D26" s="11" t="str" cm="1">
         <f t="array" ref="D26">IF(IFERROR(IFERROR(INDEX(L:L,$F26),INDEX(R:R,$G26)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F26),INDEX(R:R,$G26)),"-"))</f>
@@ -3549,7 +3429,7 @@
         <v>#N/A</v>
       </c>
       <c r="G26" s="1" t="e">
-        <f>MATCH(E26,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I26" s="8" t="s">
@@ -3577,23 +3457,23 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:18" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="12" t="str" cm="1">
+      <c r="B27" s="11" t="str" cm="1">
         <f t="array" ref="B27">IF(IFERROR(IFERROR(INDEX(J:J,$F27),INDEX(Q:Q,$G27)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F27),INDEX(Q:Q,$G27)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C27" s="13" t="str" cm="1">
+      <c r="C27" s="12" t="str" cm="1">
         <f t="array" ref="C27">IF(IFERROR(IFERROR(INDEX(K:K,$F27),INDEX(O:O,$G27)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F27),INDEX(O:O,$G27)),"-"))</f>
         <v>Regulatory Measure Type (Permit Type)</v>
       </c>
-      <c r="D27" s="12" t="str" cm="1">
+      <c r="D27" s="11" t="str" cm="1">
         <f t="array" ref="D27">IF(IFERROR(IFERROR(INDEX(L:L,$F27),INDEX(R:R,$G27)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F27),INDEX(R:R,$G27)),"-"))</f>
@@ -3607,10 +3487,10 @@
         <v>2</v>
       </c>
       <c r="G27" s="1" t="e">
-        <f>MATCH(E27,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I27" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I27" s="13" t="s">
         <v>57</v>
       </c>
       <c r="J27" s="5"/>
@@ -3629,29 +3509,29 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:18" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="12" t="str" cm="1">
+      <c r="B28" s="11" t="str" cm="1">
         <f t="array" ref="B28">IF(IFERROR(IFERROR(INDEX(J:J,$F28),INDEX(Q:Q,$G28)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F28),INDEX(Q:Q,$G28)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C28" s="13" t="str" cm="1">
+      <c r="C28" s="12" t="str" cm="1">
         <f t="array" ref="C28">IF(IFERROR(IFERROR(INDEX(K:K,$F28),INDEX(O:O,$G28)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F28),INDEX(O:O,$G28)),"-"))</f>
         <v>Regional Water Board number</v>
       </c>
-      <c r="D28" s="12" t="str" cm="1">
+      <c r="D28" s="11" t="str" cm="1">
         <f t="array" ref="D28">IF(IFERROR(IFERROR(INDEX(L:L,$F28),INDEX(R:R,$G28)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F28),INDEX(R:R,$G28)),"-"))</f>
         <v>Regional Water Quality Control Board office that has primary responsibility for regulation of the facility: “1” - North Coast; “2” - San Francisco Bay; “3” - Central Coast; “4” - Los Angeles; “5F” - Central Valley (Fresno); “5R” - Central Valley (Redding); “5S” - Central Valley (Sacramento); “6” - Lahontan; “7” - Colorado River; “8” - Santa Ana; “9” - San Diego.</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1">
@@ -3659,10 +3539,10 @@
         <v>8</v>
       </c>
       <c r="G28" s="1" t="e">
-        <f>MATCH(E28,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I28" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I28" s="13" t="s">
         <v>58</v>
       </c>
       <c r="J28" s="5"/>
@@ -3681,23 +3561,23 @@
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
+    <row r="29" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="12" t="str" cm="1">
+      <c r="B29" s="11" t="str" cm="1">
         <f t="array" ref="B29">IF(IFERROR(IFERROR(INDEX(J:J,$F29),INDEX(Q:Q,$G29)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F29),INDEX(Q:Q,$G29)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C29" s="13" t="str" cm="1">
+      <c r="C29" s="12" t="str" cm="1">
         <f t="array" ref="C29">IF(IFERROR(IFERROR(INDEX(K:K,$F29),INDEX(O:O,$G29)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F29),INDEX(O:O,$G29)),"-"))</f>
         <v>Facility/Site County</v>
       </c>
-      <c r="D29" s="12" t="str" cm="1">
+      <c r="D29" s="11" t="str" cm="1">
         <f t="array" ref="D29">IF(IFERROR(IFERROR(INDEX(L:L,$F29),INDEX(R:R,$G29)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F29),INDEX(R:R,$G29)),"-"))</f>
@@ -3711,10 +3591,10 @@
         <v>9</v>
       </c>
       <c r="G29" s="1" t="e">
-        <f>MATCH(E29,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I29" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I29" s="13" t="s">
         <v>59</v>
       </c>
       <c r="J29" s="5"/>
@@ -3733,23 +3613,23 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="12" t="str" cm="1">
+      <c r="B30" s="11" t="str" cm="1">
         <f t="array" ref="B30">IF(IFERROR(IFERROR(INDEX(J:J,$F30),INDEX(Q:Q,$G30)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F30),INDEX(Q:Q,$G30)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C30" s="13" t="str" cm="1">
+      <c r="C30" s="12" t="str" cm="1">
         <f t="array" ref="C30">IF(IFERROR(IFERROR(INDEX(K:K,$F30),INDEX(O:O,$G30)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F30),INDEX(O:O,$G30)),"-"))</f>
         <v>Facility/Site Name</v>
       </c>
-      <c r="D30" s="12" t="str" cm="1">
+      <c r="D30" s="11" t="str" cm="1">
         <f t="array" ref="D30">IF(IFERROR(IFERROR(INDEX(L:L,$F30),INDEX(R:R,$G30)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F30),INDEX(R:R,$G30)),"-"))</f>
@@ -3763,7 +3643,7 @@
         <v>11</v>
       </c>
       <c r="G30" s="1">
-        <f>MATCH(E30,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I30" s="8" t="s">
@@ -3791,23 +3671,23 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="12" t="str" cm="1">
+      <c r="B31" s="11" t="str" cm="1">
         <f t="array" ref="B31">IF(IFERROR(IFERROR(INDEX(J:J,$F31),INDEX(Q:Q,$G31)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F31),INDEX(Q:Q,$G31)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C31" s="13" t="str" cm="1">
+      <c r="C31" s="12" t="str" cm="1">
         <f t="array" ref="C31">IF(IFERROR(IFERROR(INDEX(K:K,$F31),INDEX(O:O,$G31)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F31),INDEX(O:O,$G31)),"-"))</f>
         <v>Facility/Site Address</v>
       </c>
-      <c r="D31" s="12" t="str" cm="1">
+      <c r="D31" s="11" t="str" cm="1">
         <f t="array" ref="D31">IF(IFERROR(IFERROR(INDEX(L:L,$F31),INDEX(R:R,$G31)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F31),INDEX(R:R,$G31)),"-"))</f>
@@ -3821,7 +3701,7 @@
         <v>12</v>
       </c>
       <c r="G31" s="1" t="e">
-        <f>MATCH(E31,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I31" s="8" t="s">
@@ -3849,23 +3729,23 @@
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="12" t="str" cm="1">
+      <c r="B32" s="11" t="str" cm="1">
         <f t="array" ref="B32">IF(IFERROR(IFERROR(INDEX(J:J,$F32),INDEX(Q:Q,$G32)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F32),INDEX(Q:Q,$G32)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C32" s="13" t="str" cm="1">
+      <c r="C32" s="12" t="str" cm="1">
         <f t="array" ref="C32">IF(IFERROR(IFERROR(INDEX(K:K,$F32),INDEX(O:O,$G32)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F32),INDEX(O:O,$G32)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D32" s="12" t="str" cm="1">
+      <c r="D32" s="11" t="str" cm="1">
         <f t="array" ref="D32">IF(IFERROR(IFERROR(INDEX(L:L,$F32),INDEX(R:R,$G32)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F32),INDEX(R:R,$G32)),"-"))</f>
@@ -3879,7 +3759,7 @@
         <v>13</v>
       </c>
       <c r="G32" s="1" t="e">
-        <f>MATCH(E32,P:P,0)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="I32" s="8" t="s">
@@ -3907,23 +3787,23 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
+    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="12" t="str" cm="1">
+      <c r="B33" s="11" t="str" cm="1">
         <f t="array" ref="B33">IF(IFERROR(IFERROR(INDEX(J:J,$F33),INDEX(Q:Q,$G33)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F33),INDEX(Q:Q,$G33)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C33" s="13" t="str" cm="1">
+      <c r="C33" s="12" t="str" cm="1">
         <f t="array" ref="C33">IF(IFERROR(IFERROR(INDEX(K:K,$F33),INDEX(O:O,$G33)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F33),INDEX(O:O,$G33)),"-"))</f>
         <v>Facility/Site City</v>
       </c>
-      <c r="D33" s="12" t="str" cm="1">
+      <c r="D33" s="11" t="str" cm="1">
         <f t="array" ref="D33">IF(IFERROR(IFERROR(INDEX(L:L,$F33),INDEX(R:R,$G33)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F33),INDEX(R:R,$G33)),"-"))</f>
@@ -3937,10 +3817,10 @@
         <v>14</v>
       </c>
       <c r="G33" s="1" t="e">
-        <f>MATCH(E33,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I33" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I33" s="13" t="s">
         <v>67</v>
       </c>
       <c r="J33" s="5"/>
@@ -3959,23 +3839,23 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="12" t="str" cm="1">
+      <c r="B34" s="11" t="str" cm="1">
         <f t="array" ref="B34">IF(IFERROR(IFERROR(INDEX(J:J,$F34),INDEX(Q:Q,$G34)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F34),INDEX(Q:Q,$G34)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C34" s="13" t="str" cm="1">
+      <c r="C34" s="12" t="str" cm="1">
         <f t="array" ref="C34">IF(IFERROR(IFERROR(INDEX(K:K,$F34),INDEX(O:O,$G34)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F34),INDEX(O:O,$G34)),"-"))</f>
         <v>Facility/Site State</v>
       </c>
-      <c r="D34" s="12" t="str" cm="1">
+      <c r="D34" s="11" t="str" cm="1">
         <f t="array" ref="D34">IF(IFERROR(IFERROR(INDEX(L:L,$F34),INDEX(R:R,$G34)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F34),INDEX(R:R,$G34)),"-"))</f>
@@ -3989,33 +3869,33 @@
         <v>15</v>
       </c>
       <c r="G34" s="1" t="e">
-        <f>MATCH(E34,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I34" s="15" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I34" s="14" t="s">
         <v>68</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
+    <row r="35" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="12" t="str" cm="1">
+      <c r="B35" s="11" t="str" cm="1">
         <f t="array" ref="B35">IF(IFERROR(IFERROR(INDEX(J:J,$F35),INDEX(Q:Q,$G35)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F35),INDEX(Q:Q,$G35)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C35" s="13" t="str" cm="1">
+      <c r="C35" s="12" t="str" cm="1">
         <f t="array" ref="C35">IF(IFERROR(IFERROR(INDEX(K:K,$F35),INDEX(O:O,$G35)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F35),INDEX(O:O,$G35)),"-"))</f>
         <v>Facility/Site Zip</v>
       </c>
-      <c r="D35" s="12" t="str" cm="1">
+      <c r="D35" s="11" t="str" cm="1">
         <f t="array" ref="D35">IF(IFERROR(IFERROR(INDEX(L:L,$F35),INDEX(R:R,$G35)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F35),INDEX(R:R,$G35)),"-"))</f>
@@ -4029,33 +3909,33 @@
         <v>16</v>
       </c>
       <c r="G35" s="1" t="e">
-        <f>MATCH(E35,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I35" s="15" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I35" s="14" t="s">
         <v>69</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="12" t="str" cm="1">
+      <c r="B36" s="11" t="str" cm="1">
         <f t="array" ref="B36">IF(IFERROR(IFERROR(INDEX(J:J,$F36),INDEX(Q:Q,$G36)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F36),INDEX(Q:Q,$G36)),"-"))</f>
         <v>Number</v>
       </c>
-      <c r="C36" s="13" t="str" cm="1">
+      <c r="C36" s="12" t="str" cm="1">
         <f t="array" ref="C36">IF(IFERROR(IFERROR(INDEX(K:K,$F36),INDEX(O:O,$G36)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F36),INDEX(O:O,$G36)),"-"))</f>
         <v>Latitude</v>
       </c>
-      <c r="D36" s="12" t="str" cm="1">
+      <c r="D36" s="11" t="str" cm="1">
         <f t="array" ref="D36">IF(IFERROR(IFERROR(INDEX(L:L,$F36),INDEX(R:R,$G36)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F36),INDEX(R:R,$G36)),"-"))</f>
@@ -4065,37 +3945,37 @@
         <v>43</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" ref="F36:F44" si="1">MATCH(E36,I:I,0)</f>
+        <f t="shared" ref="F36:F43" si="2">MATCH(E36,I:I,0)</f>
         <v>17</v>
       </c>
       <c r="G36" s="1" t="e">
-        <f>MATCH(E36,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I36" s="15" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I36" s="14" t="s">
         <v>70</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+    <row r="37" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="12" t="str" cm="1">
+      <c r="B37" s="11" t="str" cm="1">
         <f t="array" ref="B37">IF(IFERROR(IFERROR(INDEX(J:J,$F37),INDEX(Q:Q,$G37)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F37),INDEX(Q:Q,$G37)),"-"))</f>
         <v>Number</v>
       </c>
-      <c r="C37" s="13" t="str" cm="1">
+      <c r="C37" s="12" t="str" cm="1">
         <f t="array" ref="C37">IF(IFERROR(IFERROR(INDEX(K:K,$F37),INDEX(O:O,$G37)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F37),INDEX(O:O,$G37)),"-"))</f>
         <v>Longitude</v>
       </c>
-      <c r="D37" s="12" t="str" cm="1">
+      <c r="D37" s="11" t="str" cm="1">
         <f t="array" ref="D37">IF(IFERROR(IFERROR(INDEX(L:L,$F37),INDEX(R:R,$G37)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F37),INDEX(R:R,$G37)),"-"))</f>
@@ -4105,37 +3985,37 @@
         <v>46</v>
       </c>
       <c r="F37" s="1">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="G37" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="G37" s="1" t="e">
-        <f>MATCH(E37,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I37" s="15" t="s">
+        <v>#N/A</v>
+      </c>
+      <c r="I37" s="14" t="s">
         <v>71</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
+    <row r="38" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="12" t="str" cm="1">
+      <c r="B38" s="11" t="str" cm="1">
         <f t="array" ref="B38">IF(IFERROR(IFERROR(INDEX(J:J,$F38),INDEX(Q:Q,$G38)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F38),INDEX(Q:Q,$G38)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C38" s="13" t="str" cm="1">
+      <c r="C38" s="12" t="str" cm="1">
         <f t="array" ref="C38">IF(IFERROR(IFERROR(INDEX(K:K,$F38),INDEX(O:O,$G38)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F38),INDEX(O:O,$G38)),"-"))</f>
         <v>Facility/Site County</v>
       </c>
-      <c r="D38" s="12" t="str" cm="1">
+      <c r="D38" s="11" t="str" cm="1">
         <f t="array" ref="D38">IF(IFERROR(IFERROR(INDEX(L:L,$F38),INDEX(R:R,$G38)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F38),INDEX(R:R,$G38)),"-"))</f>
@@ -4145,37 +4025,37 @@
         <v>48</v>
       </c>
       <c r="F38" s="1">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="G38" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="G38" s="1" t="e">
-        <f>MATCH(E38,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I38" s="15" t="s">
+        <v>#N/A</v>
+      </c>
+      <c r="I38" s="14" t="s">
         <v>72</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
+    <row r="39" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="12" t="str" cm="1">
+      <c r="B39" s="11" t="str" cm="1">
         <f t="array" ref="B39">IF(IFERROR(IFERROR(INDEX(J:J,$F39),INDEX(Q:Q,$G39)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F39),INDEX(Q:Q,$G39)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C39" s="13" t="str" cm="1">
+      <c r="C39" s="12" t="str" cm="1">
         <f t="array" ref="C39">IF(IFERROR(IFERROR(INDEX(K:K,$F39),INDEX(O:O,$G39)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F39),INDEX(O:O,$G39)),"-"))</f>
         <v>Facility/Site Size</v>
       </c>
-      <c r="D39" s="12" t="str" cm="1">
+      <c r="D39" s="11" t="str" cm="1">
         <f t="array" ref="D39">IF(IFERROR(IFERROR(INDEX(L:L,$F39),INDEX(R:R,$G39)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F39),INDEX(R:R,$G39)),"-"))</f>
@@ -4185,31 +4065,31 @@
         <v>54</v>
       </c>
       <c r="F39" s="1">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G39" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="G39" s="1" t="e">
-        <f>MATCH(E39,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="12" t="str" cm="1">
+      <c r="B40" s="11" t="str" cm="1">
         <f t="array" ref="B40">IF(IFERROR(IFERROR(INDEX(J:J,$F40),INDEX(Q:Q,$G40)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F40),INDEX(Q:Q,$G40)),"-"))</f>
         <v>Plain Text</v>
       </c>
-      <c r="C40" s="13" t="str" cm="1">
+      <c r="C40" s="12" t="str" cm="1">
         <f t="array" ref="C40">IF(IFERROR(IFERROR(INDEX(K:K,$F40),INDEX(O:O,$G40)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F40),INDEX(O:O,$G40)),"-"))</f>
         <v>Facility/Site Size Unit</v>
       </c>
-      <c r="D40" s="12" t="str" cm="1">
+      <c r="D40" s="11" t="str" cm="1">
         <f t="array" ref="D40">IF(IFERROR(IFERROR(INDEX(L:L,$F40),INDEX(R:R,$G40)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F40),INDEX(R:R,$G40)),"-"))</f>
@@ -4219,31 +4099,31 @@
         <v>55</v>
       </c>
       <c r="F40" s="1">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="G40" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="G40" s="1" t="e">
-        <f>MATCH(E40,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="12" t="str" cm="1">
+      <c r="B41" s="11" t="str" cm="1">
         <f t="array" ref="B41">IF(IFERROR(IFERROR(INDEX(J:J,$F41),INDEX(Q:Q,$G41)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F41),INDEX(Q:Q,$G41)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C41" s="13" t="str" cm="1">
+      <c r="C41" s="12" t="str" cm="1">
         <f t="array" ref="C41">IF(IFERROR(IFERROR(INDEX(K:K,$F41),INDEX(O:O,$G41)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F41),INDEX(O:O,$G41)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D41" s="12" t="str" cm="1">
+      <c r="D41" s="11" t="str" cm="1">
         <f t="array" ref="D41">IF(IFERROR(IFERROR(INDEX(L:L,$F41),INDEX(R:R,$G41)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F41),INDEX(R:R,$G41)),"-"))</f>
@@ -4253,31 +4133,31 @@
         <v>67</v>
       </c>
       <c r="F41" s="1">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="G41" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="G41" s="1" t="e">
-        <f>MATCH(E41,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="12" t="str" cm="1">
+      <c r="B42" s="11" t="str" cm="1">
         <f t="array" ref="B42">IF(IFERROR(IFERROR(INDEX(J:J,$F42),INDEX(Q:Q,$G42)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F42),INDEX(Q:Q,$G42)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C42" s="13" t="str" cm="1">
+      <c r="C42" s="12" t="str" cm="1">
         <f t="array" ref="C42">IF(IFERROR(IFERROR(INDEX(K:K,$F42),INDEX(O:O,$G42)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F42),INDEX(O:O,$G42)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D42" s="12" t="str" cm="1">
+      <c r="D42" s="11" t="str" cm="1">
         <f t="array" ref="D42">IF(IFERROR(IFERROR(INDEX(L:L,$F42),INDEX(R:R,$G42)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F42),INDEX(R:R,$G42)),"-"))</f>
@@ -4287,31 +4167,31 @@
         <v>68</v>
       </c>
       <c r="F42" s="1">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="G42" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="G42" s="1" t="e">
-        <f>MATCH(E42,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="12" t="str" cm="1">
+      <c r="B43" s="11" t="str" cm="1">
         <f t="array" ref="B43">IF(IFERROR(IFERROR(INDEX(J:J,$F43),INDEX(Q:Q,$G43)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(J:J,$F43),INDEX(Q:Q,$G43)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="C43" s="13" t="str" cm="1">
+      <c r="C43" s="12" t="str" cm="1">
         <f t="array" ref="C43">IF(IFERROR(IFERROR(INDEX(K:K,$F43),INDEX(O:O,$G43)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(K:K,$F43),INDEX(O:O,$G43)),"-"))</f>
         <v>-</v>
       </c>
-      <c r="D43" s="12" t="str" cm="1">
+      <c r="D43" s="11" t="str" cm="1">
         <f t="array" ref="D43">IF(IFERROR(IFERROR(INDEX(L:L,$F43),INDEX(R:R,$G43)),"-")=0,
 "-",
 IFERROR(IFERROR(INDEX(L:L,$F43),INDEX(R:R,$G43)),"-"))</f>
@@ -4321,15 +4201,15 @@
         <v>69</v>
       </c>
       <c r="F43" s="1">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="G43" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G43" s="1" t="e">
-        <f>MATCH(E43,P:P,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E44"/>
     </row>
   </sheetData>

</xml_diff>